<commit_message>
continue from tag components
</commit_message>
<xml_diff>
--- a/Guidance/Data_design.XLSX
+++ b/Guidance/Data_design.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ELTE IK\7_felev_local\Szakdolgozat\Here-To-Slay\Guidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BB108F-7125-44FE-B75E-0E2BB8D2296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D5F36B-CB46-4865-9C1D-99403EAEE6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>Data</t>
   </si>
@@ -161,9 +161,6 @@
     <t>OnRollForHero</t>
   </si>
   <si>
-    <t>Ability</t>
-  </si>
-  <si>
     <t>48 hero cards</t>
   </si>
   <si>
@@ -171,55 +168,197 @@
   </si>
   <si>
     <t>Effect[]</t>
+  </si>
+  <si>
+    <t>BaseClass</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>CurrentClass</t>
+  </si>
+  <si>
+    <t>OnUnequipTool (masks)</t>
+  </si>
+  <si>
+    <t>Once on init
+OnEquipTool (masks)
+OnUnequipTool (masks)</t>
+  </si>
+  <si>
+    <t>Display class to player
+Have info on which class card reverts to when mask is removed</t>
+  </si>
+  <si>
+    <t>OnCheckWinCondition
+OnHeroOnFieldWithClass(type)
+OnMonsterAttack</t>
+  </si>
+  <si>
+    <t>win condition
+some hero effects require certain classes present on field
+Monster attacks require presence of certain classes on field</t>
+  </si>
+  <si>
+    <t>EquippedItemID</t>
+  </si>
+  <si>
+    <t>OnEquipTool
+OnUnequipTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OnRollForHero
+OnSuccessfulRollForHero
+OnUnsuccessfulRollForHero</t>
   </si>
   <si>
     <t>Once on init
 OnEquipTool
 OnUnequipTool
+OnSlayMonster
+OnMoveToPlayer - when card becomes owned by the player</t>
+  </si>
+  <si>
+    <t>When equipping hero changes decktag
+When targeted by "unequip" effects</t>
+  </si>
+  <si>
+    <t>Equipping items modifies hero ability
+Some effects target equipped tools
+Tools usually move along with the equipping hero (e.g. during destroy, steal etc.)</t>
+  </si>
+  <si>
+    <t>sActivated</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI update: hero card "glows" when True
+When targeted by player/AI
+</t>
+  </si>
+  <si>
+    <t>OnActivateHero
+OnTurnStart
+Certain effects instantly reactivate hero</t>
+  </si>
+  <si>
+    <t>Only relevant for hero cards on field.
+Helps tracking the 1 hero card activation limit per turn</t>
+  </si>
+  <si>
+    <t>LeaderClass</t>
+  </si>
+  <si>
+    <t>6 leader hero cards</t>
+  </si>
+  <si>
+    <t>once on init</t>
+  </si>
+  <si>
+    <t>HeroAbility</t>
+  </si>
+  <si>
+    <t>ItemAbility</t>
+  </si>
+  <si>
+    <t>Once on init
+OnEquipTool
+OnUnequipTool</t>
+  </si>
+  <si>
+    <t>Modifies/Adds abilities to equipped hero cards</t>
+  </si>
+  <si>
+    <t>15 item cards</t>
+  </si>
+  <si>
+    <t>SpellAbility</t>
+  </si>
+  <si>
+    <t>13 spell cards</t>
+  </si>
+  <si>
+    <t>once on init
+OnMoveToPlayer
 OnSlayMonster</t>
   </si>
   <si>
-    <t>OnSuccessfulRollForHero
-OnUnsuccessfulRollForHero</t>
-  </si>
-  <si>
-    <t>BaseClass</t>
-  </si>
-  <si>
-    <t>enum</t>
-  </si>
-  <si>
-    <t>CurrentClass</t>
-  </si>
-  <si>
-    <t>OnUnequipTool (masks)</t>
-  </si>
-  <si>
-    <t>Once on init
-OnEquipTool (masks)
-OnUnequipTool (masks)</t>
-  </si>
-  <si>
-    <t>Display class to player
-Have info on which class card reverts to when mask is removed</t>
-  </si>
-  <si>
-    <t>OnCheckWinCondition
-OnHeroOnFieldWithClass(type)
-OnMonsterAttack</t>
-  </si>
-  <si>
-    <t>win condition
-some hero effects require certain classes present on field
-Monster attacks require presence of certain classes on field</t>
+    <t>ModValues</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>Provide instructions for resolving spellcard effect</t>
+  </si>
+  <si>
+    <t>25 modifier cards</t>
+  </si>
+  <si>
+    <t>OnPlaySpell</t>
+  </si>
+  <si>
+    <t>ModifierAbility</t>
+  </si>
+  <si>
+    <t>OnPlayModifier</t>
+  </si>
+  <si>
+    <t>Possible modifying values on dice roll
+If difficult, start out with 1 possible value instead of 2</t>
+  </si>
+  <si>
+    <t>Certain monsters and leader heroes add extra effects to modifiers</t>
+  </si>
+  <si>
+    <t>ChallengeAbility</t>
+  </si>
+  <si>
+    <t>14 challengeCards</t>
+  </si>
+  <si>
+    <t>OnPlayChallenge</t>
+  </si>
+  <si>
+    <t>Certain monsters and leader heroes add extra effects to challenges</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>On certain hero abilities triggering</t>
+  </si>
+  <si>
+    <t>Some hand steal effects allow an additional steal based on stolen card type</t>
+  </si>
+  <si>
+    <t>DrawDeckTag</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>cards in draw pile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,11 +386,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -270,8 +410,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52A2D346-78F6-4648-BE76-128E00F5A338}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11" xr:uid="{52A2D346-78F6-4648-BE76-128E00F5A338}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52A2D346-78F6-4648-BE76-128E00F5A338}" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0">
+  <autoFilter ref="A1:F20" xr:uid="{52A2D346-78F6-4648-BE76-128E00F5A338}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{58EAABF2-92EB-4963-A338-9ADF57AD8EC4}" name="Data"/>
     <tableColumn id="2" xr3:uid="{F4D0D957-349D-49F7-82BE-A6355FD2AF27}" name="Type"/>
@@ -547,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,33 +786,27 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4">
-        <v>48</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -687,135 +821,332 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <f>SUM(I2:I9)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9">
-        <f>SUM(I2:I8)</f>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>51</v>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>